<commit_message>
Jupyter Notebooks' data extraction flow complete
</commit_message>
<xml_diff>
--- a/resources/jupyter.xlsx
+++ b/resources/jupyter.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -869,6 +869,341 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>WillKoehrsen</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Data-Analysis</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>42809.80076388889</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>44231.51909722222</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>376839</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Jupyter Notebook</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>6</v>
+      </c>
+      <c r="I7" t="n">
+        <v>4</v>
+      </c>
+      <c r="J7" t="n">
+        <v>350</v>
+      </c>
+      <c r="K7" t="n">
+        <v>4051</v>
+      </c>
+      <c r="L7" t="n">
+        <v>3285</v>
+      </c>
+      <c r="M7" t="n">
+        <v>56</v>
+      </c>
+      <c r="N7" t="n">
+        <v>367</v>
+      </c>
+      <c r="O7" t="n">
+        <v>15</v>
+      </c>
+      <c r="P7" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>Data Science Using Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>microsoft</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>tensorwatch</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>43600.35386574074</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>44299.40557870371</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>22242</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Jupyter Notebook</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>3</v>
+      </c>
+      <c r="I8" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J8" t="n">
+        <v>104</v>
+      </c>
+      <c r="K8" t="n">
+        <v>3182</v>
+      </c>
+      <c r="L8" t="n">
+        <v>346</v>
+      </c>
+      <c r="M8" t="n">
+        <v>65</v>
+      </c>
+      <c r="N8" t="n">
+        <v>112</v>
+      </c>
+      <c r="O8" t="n">
+        <v>14</v>
+      </c>
+      <c r="P8" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>7</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>Debugging, monitoring and visualization for Python Machine Learning and Data Science</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>nborwankar</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>LearnDataScience</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>41481.10930555555</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>43760.41459490741</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>148439</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Jupyter Notebook</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>3</v>
+      </c>
+      <c r="I9" t="n">
+        <v>7</v>
+      </c>
+      <c r="J9" t="n">
+        <v>371</v>
+      </c>
+      <c r="K9" t="n">
+        <v>2673</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1647</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" t="n">
+        <v>64</v>
+      </c>
+      <c r="O9" t="n">
+        <v>19</v>
+      </c>
+      <c r="P9" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>Open Content for self-directed learning in data science</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ml-tooling</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ml-workspace</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>43612.70503472222</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>44480.09324074074</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>13023</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Jupyter Notebook</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>7</v>
+      </c>
+      <c r="I10" t="n">
+        <v>9</v>
+      </c>
+      <c r="J10" t="n">
+        <v>62</v>
+      </c>
+      <c r="K10" t="n">
+        <v>2287</v>
+      </c>
+      <c r="L10" t="n">
+        <v>314</v>
+      </c>
+      <c r="M10" t="n">
+        <v>73</v>
+      </c>
+      <c r="N10" t="n">
+        <v>845</v>
+      </c>
+      <c r="O10" t="n">
+        <v>29</v>
+      </c>
+      <c r="P10" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>34</v>
+      </c>
+      <c r="R10" t="n">
+        <v>4</v>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>🛠 All-in-one web-based IDE specialized for machine learning and data science.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ShuaiW</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>data-science-question-answer</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>43115.06939814815</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>44105.20944444444</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>2390</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Jupyter Notebook</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" t="n">
+        <v>2</v>
+      </c>
+      <c r="J11" t="n">
+        <v>88</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1980</v>
+      </c>
+      <c r="L11" t="n">
+        <v>603</v>
+      </c>
+      <c r="M11" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" t="n">
+        <v>17</v>
+      </c>
+      <c r="O11" t="n">
+        <v>4</v>
+      </c>
+      <c r="P11" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>A repo for data science related questions and answers</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>